<commit_message>
Update player guide tables
</commit_message>
<xml_diff>
--- a/undyingkingdoms/static/metadata/armies.xlsx
+++ b/undyingkingdoms/static/metadata/armies.xlsx
@@ -1,17 +1,286 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView activeTab="0" autoFilterDateGrouping="1" firstSheet="0" minimized="0" showHorizontalScroll="1" showSheetTabs="1" showVerticalScroll="1" tabRatio="600" visibility="visible"/>
   </bookViews>
   <sheets>
-    <sheet name="Armies" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Armies" sheetId="1" state="visible" r:id="rId1"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
 </workbook>
+</file>
+
+<file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" uniqueCount="88">
+  <si>
+    <t>Race</t>
+  </si>
+  <si>
+    <t>Base Name</t>
+  </si>
+  <si>
+    <t>Class Name</t>
+  </si>
+  <si>
+    <t>Class Name Plural</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>Trainable Per Day</t>
+  </si>
+  <si>
+    <t>Gold</t>
+  </si>
+  <si>
+    <t>Iron</t>
+  </si>
+  <si>
+    <t>Wood</t>
+  </si>
+  <si>
+    <t>Upkeep</t>
+  </si>
+  <si>
+    <t>Attack</t>
+  </si>
+  <si>
+    <t>Defence</t>
+  </si>
+  <si>
+    <t>Health</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>peasant</t>
+  </si>
+  <si>
+    <t>peasants</t>
+  </si>
+  <si>
+    <t>Unknown</t>
+  </si>
+  <si>
+    <t>soldier</t>
+  </si>
+  <si>
+    <t>soldiers</t>
+  </si>
+  <si>
+    <t>archer</t>
+  </si>
+  <si>
+    <t>archers</t>
+  </si>
+  <si>
+    <t>elite</t>
+  </si>
+  <si>
+    <t>elites</t>
+  </si>
+  <si>
+    <t>monster</t>
+  </si>
+  <si>
+    <t>monsters</t>
+  </si>
+  <si>
+    <t>Human</t>
+  </si>
+  <si>
+    <t>man-at-arms</t>
+  </si>
+  <si>
+    <t>men-at-arms</t>
+  </si>
+  <si>
+    <t>Men-at-arms can be trained extremely quickly and have low upkeep.</t>
+  </si>
+  <si>
+    <t>footman</t>
+  </si>
+  <si>
+    <t>footmen</t>
+  </si>
+  <si>
+    <t>Footmen are strong attackers.</t>
+  </si>
+  <si>
+    <t>musketeer</t>
+  </si>
+  <si>
+    <t>musketeers</t>
+  </si>
+  <si>
+    <t>Crossbowmen are excellent at defending.</t>
+  </si>
+  <si>
+    <t>knight</t>
+  </si>
+  <si>
+    <t>knights</t>
+  </si>
+  <si>
+    <t>Knights are one of the best attackers.</t>
+  </si>
+  <si>
+    <t>gryphon</t>
+  </si>
+  <si>
+    <t>gryphons</t>
+  </si>
+  <si>
+    <t>Gryphons are incredibly powerful monsters.</t>
+  </si>
+  <si>
+    <t>Elf</t>
+  </si>
+  <si>
+    <t>defender</t>
+  </si>
+  <si>
+    <t>defenders</t>
+  </si>
+  <si>
+    <t>They excel at repelling enemy armies.</t>
+  </si>
+  <si>
+    <t>ranger</t>
+  </si>
+  <si>
+    <t>rangers</t>
+  </si>
+  <si>
+    <t>Excellent offensive troops.</t>
+  </si>
+  <si>
+    <t>longbowman</t>
+  </si>
+  <si>
+    <t>longbowmen</t>
+  </si>
+  <si>
+    <t>Longbowmen are very effective at defending your county.</t>
+  </si>
+  <si>
+    <t>dragonhelm</t>
+  </si>
+  <si>
+    <t>dragonhelms</t>
+  </si>
+  <si>
+    <t>Dragonhelms are elite cavalry and incredibly adept at attacking enemy counties.</t>
+  </si>
+  <si>
+    <t>dragon</t>
+  </si>
+  <si>
+    <t>dragons</t>
+  </si>
+  <si>
+    <t>Dragons are incredibly powerful monsters.</t>
+  </si>
+  <si>
+    <t>Dwarf</t>
+  </si>
+  <si>
+    <t>miner</t>
+  </si>
+  <si>
+    <t>miners</t>
+  </si>
+  <si>
+    <t>Miners deal extra damage when attacking.</t>
+  </si>
+  <si>
+    <t>axeman</t>
+  </si>
+  <si>
+    <t>axemen</t>
+  </si>
+  <si>
+    <t>rifleman</t>
+  </si>
+  <si>
+    <t>riflemen</t>
+  </si>
+  <si>
+    <t>Dwarf riflemen are a powerful defensive force.</t>
+  </si>
+  <si>
+    <t>greybeard</t>
+  </si>
+  <si>
+    <t>greybeards</t>
+  </si>
+  <si>
+    <t>Greybeards are capable of defending, as well as attacking.</t>
+  </si>
+  <si>
+    <t>manticore</t>
+  </si>
+  <si>
+    <t>manticores</t>
+  </si>
+  <si>
+    <t>Manticores are incredibly powerful monsters.</t>
+  </si>
+  <si>
+    <t>Goblin</t>
+  </si>
+  <si>
+    <t>scout</t>
+  </si>
+  <si>
+    <t>scouts</t>
+  </si>
+  <si>
+    <t>Scouts are cheap and expendable.</t>
+  </si>
+  <si>
+    <t>berserker</t>
+  </si>
+  <si>
+    <t>berserkers</t>
+  </si>
+  <si>
+    <t>Soldiers are a solid offensive troop.</t>
+  </si>
+  <si>
+    <t>bowman</t>
+  </si>
+  <si>
+    <t>bowmen</t>
+  </si>
+  <si>
+    <t>Goblin archers are weaker than other archers but much cheaper.</t>
+  </si>
+  <si>
+    <t>wolf rider</t>
+  </si>
+  <si>
+    <t>wolf riders</t>
+  </si>
+  <si>
+    <t>In large numbers, wolf riders are incredibly powerful.</t>
+  </si>
+  <si>
+    <t>wyvern</t>
+  </si>
+  <si>
+    <t>wyverns</t>
+  </si>
+  <si>
+    <t>Wyverns are devastating to any who cross their path.</t>
+  </si>
+</sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
@@ -366,97 +635,63 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <sheetData>
-    <row r="1">
-      <c r="B1" s="1" t="inlineStr">
-        <is>
-          <t>Race</t>
-        </is>
-      </c>
-      <c r="C1" s="1" t="inlineStr">
-        <is>
-          <t>Base Name</t>
-        </is>
-      </c>
-      <c r="D1" s="1" t="inlineStr">
-        <is>
-          <t>Class Name</t>
-        </is>
-      </c>
-      <c r="E1" s="1" t="inlineStr">
-        <is>
-          <t>Class Name Plural</t>
-        </is>
-      </c>
-      <c r="F1" s="1" t="inlineStr">
-        <is>
-          <t>Total</t>
-        </is>
-      </c>
-      <c r="G1" s="1" t="inlineStr">
-        <is>
-          <t>Trainable Per Day</t>
-        </is>
-      </c>
-      <c r="H1" s="1" t="inlineStr">
-        <is>
-          <t>Gold</t>
-        </is>
-      </c>
-      <c r="I1" s="1" t="inlineStr">
-        <is>
-          <t>Iron</t>
-        </is>
-      </c>
-      <c r="J1" s="1" t="inlineStr">
-        <is>
-          <t>Wood</t>
-        </is>
-      </c>
-      <c r="K1" s="1" t="inlineStr">
-        <is>
-          <t>Upkeep</t>
-        </is>
-      </c>
-      <c r="L1" s="1" t="inlineStr">
-        <is>
-          <t>Attack</t>
-        </is>
-      </c>
-      <c r="M1" s="1" t="inlineStr">
-        <is>
-          <t>Defence</t>
-        </is>
-      </c>
-      <c r="N1" s="1" t="inlineStr">
-        <is>
-          <t>Health</t>
-        </is>
-      </c>
-      <c r="O1" s="1" t="inlineStr">
-        <is>
-          <t>Description</t>
-        </is>
-      </c>
-    </row>
-    <row r="2">
+    <row r="1" spans="1:15">
+      <c r="B1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>4</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="K1" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="L1" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="M1" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="N1" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="O1" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="2" spans="1:15">
       <c r="A2" s="1" t="n">
         <v>0</v>
       </c>
-      <c r="B2" t="inlineStr"/>
-      <c r="C2" t="inlineStr">
-        <is>
-          <t>peasant</t>
-        </is>
-      </c>
-      <c r="D2" t="inlineStr">
-        <is>
-          <t>peasant</t>
-        </is>
-      </c>
-      <c r="E2" t="inlineStr">
-        <is>
-          <t>peasants</t>
-        </is>
+      <c r="B2" t="s"/>
+      <c r="C2" t="s">
+        <v>14</v>
+      </c>
+      <c r="D2" t="s">
+        <v>14</v>
+      </c>
+      <c r="E2" t="s">
+        <v>15</v>
       </c>
       <c r="F2" t="n">
         <v>25</v>
@@ -485,31 +720,23 @@
       <c r="N2" t="n">
         <v>1</v>
       </c>
-      <c r="O2" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="3">
+      <c r="O2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:15">
       <c r="A3" s="1" t="n">
         <v>1</v>
       </c>
-      <c r="B3" t="inlineStr"/>
-      <c r="C3" t="inlineStr">
-        <is>
-          <t>soldier</t>
-        </is>
-      </c>
-      <c r="D3" t="inlineStr">
-        <is>
-          <t>soldier</t>
-        </is>
-      </c>
-      <c r="E3" t="inlineStr">
-        <is>
-          <t>soldiers</t>
-        </is>
+      <c r="B3" t="s"/>
+      <c r="C3" t="s">
+        <v>17</v>
+      </c>
+      <c r="D3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" t="s">
+        <v>18</v>
       </c>
       <c r="F3" t="n">
         <v>0</v>
@@ -538,31 +765,23 @@
       <c r="N3" t="n">
         <v>3</v>
       </c>
-      <c r="O3" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="4">
+      <c r="O3" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="4" spans="1:15">
       <c r="A4" s="1" t="n">
         <v>2</v>
       </c>
-      <c r="B4" t="inlineStr"/>
-      <c r="C4" t="inlineStr">
-        <is>
-          <t>archer</t>
-        </is>
-      </c>
-      <c r="D4" t="inlineStr">
-        <is>
-          <t>archer</t>
-        </is>
-      </c>
-      <c r="E4" t="inlineStr">
-        <is>
-          <t>archers</t>
-        </is>
+      <c r="B4" t="s"/>
+      <c r="C4" t="s">
+        <v>19</v>
+      </c>
+      <c r="D4" t="s">
+        <v>19</v>
+      </c>
+      <c r="E4" t="s">
+        <v>20</v>
       </c>
       <c r="F4" t="n">
         <v>30</v>
@@ -591,31 +810,23 @@
       <c r="N4" t="n">
         <v>3</v>
       </c>
-      <c r="O4" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="5">
+      <c r="O4" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="5" spans="1:15">
       <c r="A5" s="1" t="n">
         <v>3</v>
       </c>
-      <c r="B5" t="inlineStr"/>
-      <c r="C5" t="inlineStr">
-        <is>
-          <t>elite</t>
-        </is>
-      </c>
-      <c r="D5" t="inlineStr">
-        <is>
-          <t>elite</t>
-        </is>
-      </c>
-      <c r="E5" t="inlineStr">
-        <is>
-          <t>elites</t>
-        </is>
+      <c r="B5" t="s"/>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>21</v>
+      </c>
+      <c r="E5" t="s">
+        <v>22</v>
       </c>
       <c r="F5" t="n">
         <v>0</v>
@@ -644,31 +855,23 @@
       <c r="N5" t="n">
         <v>6</v>
       </c>
-      <c r="O5" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="6">
+      <c r="O5" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="6" spans="1:15">
       <c r="A6" s="1" t="n">
         <v>4</v>
       </c>
-      <c r="B6" t="inlineStr"/>
-      <c r="C6" t="inlineStr">
-        <is>
-          <t>monster</t>
-        </is>
-      </c>
-      <c r="D6" t="inlineStr">
-        <is>
-          <t>monster</t>
-        </is>
-      </c>
-      <c r="E6" t="inlineStr">
-        <is>
-          <t>monsters</t>
-        </is>
+      <c r="B6" t="s"/>
+      <c r="C6" t="s">
+        <v>23</v>
+      </c>
+      <c r="D6" t="s">
+        <v>23</v>
+      </c>
+      <c r="E6" t="s">
+        <v>24</v>
       </c>
       <c r="F6" t="n">
         <v>0</v>
@@ -697,35 +900,25 @@
       <c r="N6" t="n">
         <v>25</v>
       </c>
-      <c r="O6" t="inlineStr">
-        <is>
-          <t>Unknown</t>
-        </is>
-      </c>
-    </row>
-    <row r="7">
+      <c r="O6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="7" spans="1:15">
       <c r="A7" s="1" t="n">
         <v>5</v>
       </c>
-      <c r="B7" t="inlineStr">
-        <is>
-          <t>Human</t>
-        </is>
-      </c>
-      <c r="C7" t="inlineStr">
-        <is>
-          <t>peasant</t>
-        </is>
-      </c>
-      <c r="D7" t="inlineStr">
-        <is>
-          <t>man-at-arms</t>
-        </is>
-      </c>
-      <c r="E7" t="inlineStr">
-        <is>
-          <t>men-at-arms</t>
-        </is>
+      <c r="B7" t="s">
+        <v>25</v>
+      </c>
+      <c r="C7" t="s">
+        <v>14</v>
+      </c>
+      <c r="D7" t="s">
+        <v>26</v>
+      </c>
+      <c r="E7" t="s">
+        <v>27</v>
       </c>
       <c r="F7" t="n">
         <v>25</v>
@@ -754,35 +947,25 @@
       <c r="N7" t="n">
         <v>1</v>
       </c>
-      <c r="O7" t="inlineStr">
-        <is>
-          <t>Men-at-arms can be trained extremely quickly and have low upkeep.</t>
-        </is>
-      </c>
-    </row>
-    <row r="8">
+      <c r="O7" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="8" spans="1:15">
       <c r="A8" s="1" t="n">
         <v>6</v>
       </c>
-      <c r="B8" t="inlineStr">
-        <is>
-          <t>Human</t>
-        </is>
-      </c>
-      <c r="C8" t="inlineStr">
-        <is>
-          <t>soldier</t>
-        </is>
-      </c>
-      <c r="D8" t="inlineStr">
-        <is>
-          <t>footman</t>
-        </is>
-      </c>
-      <c r="E8" t="inlineStr">
-        <is>
-          <t>footmen</t>
-        </is>
+      <c r="B8" t="s">
+        <v>25</v>
+      </c>
+      <c r="C8" t="s">
+        <v>17</v>
+      </c>
+      <c r="D8" t="s">
+        <v>29</v>
+      </c>
+      <c r="E8" t="s">
+        <v>30</v>
       </c>
       <c r="F8" t="n">
         <v>0</v>
@@ -811,35 +994,25 @@
       <c r="N8" t="n">
         <v>3</v>
       </c>
-      <c r="O8" t="inlineStr">
-        <is>
-          <t>Footmen are strong attackers.</t>
-        </is>
-      </c>
-    </row>
-    <row r="9">
+      <c r="O8" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="9" spans="1:15">
       <c r="A9" s="1" t="n">
         <v>7</v>
       </c>
-      <c r="B9" t="inlineStr">
-        <is>
-          <t>Human</t>
-        </is>
-      </c>
-      <c r="C9" t="inlineStr">
-        <is>
-          <t>archer</t>
-        </is>
-      </c>
-      <c r="D9" t="inlineStr">
-        <is>
-          <t>musketeer</t>
-        </is>
-      </c>
-      <c r="E9" t="inlineStr">
-        <is>
-          <t>musketeers</t>
-        </is>
+      <c r="B9" t="s">
+        <v>25</v>
+      </c>
+      <c r="C9" t="s">
+        <v>19</v>
+      </c>
+      <c r="D9" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" t="s">
+        <v>33</v>
       </c>
       <c r="F9" t="n">
         <v>30</v>
@@ -868,35 +1041,25 @@
       <c r="N9" t="n">
         <v>3</v>
       </c>
-      <c r="O9" t="inlineStr">
-        <is>
-          <t>Crossbowmen are excellent at defending.</t>
-        </is>
-      </c>
-    </row>
-    <row r="10">
+      <c r="O9" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="10" spans="1:15">
       <c r="A10" s="1" t="n">
         <v>8</v>
       </c>
-      <c r="B10" t="inlineStr">
-        <is>
-          <t>Human</t>
-        </is>
-      </c>
-      <c r="C10" t="inlineStr">
-        <is>
-          <t>elite</t>
-        </is>
-      </c>
-      <c r="D10" t="inlineStr">
-        <is>
-          <t>knight</t>
-        </is>
-      </c>
-      <c r="E10" t="inlineStr">
-        <is>
-          <t>knights</t>
-        </is>
+      <c r="B10" t="s">
+        <v>25</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>35</v>
+      </c>
+      <c r="E10" t="s">
+        <v>36</v>
       </c>
       <c r="F10" t="n">
         <v>0</v>
@@ -925,35 +1088,25 @@
       <c r="N10" t="n">
         <v>6</v>
       </c>
-      <c r="O10" t="inlineStr">
-        <is>
-          <t>Knights are one of the best attackers.</t>
-        </is>
-      </c>
-    </row>
-    <row r="11">
+      <c r="O10" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="11" spans="1:15">
       <c r="A11" s="1" t="n">
         <v>9</v>
       </c>
-      <c r="B11" t="inlineStr">
-        <is>
-          <t>Human</t>
-        </is>
-      </c>
-      <c r="C11" t="inlineStr">
-        <is>
-          <t>monster</t>
-        </is>
-      </c>
-      <c r="D11" t="inlineStr">
-        <is>
-          <t>gryphon</t>
-        </is>
-      </c>
-      <c r="E11" t="inlineStr">
-        <is>
-          <t>gryphons</t>
-        </is>
+      <c r="B11" t="s">
+        <v>25</v>
+      </c>
+      <c r="C11" t="s">
+        <v>23</v>
+      </c>
+      <c r="D11" t="s">
+        <v>38</v>
+      </c>
+      <c r="E11" t="s">
+        <v>39</v>
       </c>
       <c r="F11" t="n">
         <v>0</v>
@@ -982,35 +1135,25 @@
       <c r="N11" t="n">
         <v>25</v>
       </c>
-      <c r="O11" t="inlineStr">
-        <is>
-          <t>Gryphons are incredibly powerful monsters.</t>
-        </is>
-      </c>
-    </row>
-    <row r="12">
+      <c r="O11" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="12" spans="1:15">
       <c r="A12" s="1" t="n">
         <v>10</v>
       </c>
-      <c r="B12" t="inlineStr">
-        <is>
-          <t>Elf</t>
-        </is>
-      </c>
-      <c r="C12" t="inlineStr">
-        <is>
-          <t>peasant</t>
-        </is>
-      </c>
-      <c r="D12" t="inlineStr">
-        <is>
-          <t>defender</t>
-        </is>
-      </c>
-      <c r="E12" t="inlineStr">
-        <is>
-          <t>defenders</t>
-        </is>
+      <c r="B12" t="s">
+        <v>41</v>
+      </c>
+      <c r="C12" t="s">
+        <v>14</v>
+      </c>
+      <c r="D12" t="s">
+        <v>42</v>
+      </c>
+      <c r="E12" t="s">
+        <v>43</v>
       </c>
       <c r="F12" t="n">
         <v>25</v>
@@ -1025,7 +1168,7 @@
         <v>2</v>
       </c>
       <c r="J12" t="n">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="K12" t="n">
         <v>5</v>
@@ -1039,35 +1182,25 @@
       <c r="N12" t="n">
         <v>1</v>
       </c>
-      <c r="O12" t="inlineStr">
-        <is>
-          <t>They excel at repelling enemy armies.</t>
-        </is>
-      </c>
-    </row>
-    <row r="13">
+      <c r="O12" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="13" spans="1:15">
       <c r="A13" s="1" t="n">
         <v>11</v>
       </c>
-      <c r="B13" t="inlineStr">
-        <is>
-          <t>Elf</t>
-        </is>
-      </c>
-      <c r="C13" t="inlineStr">
-        <is>
-          <t>soldier</t>
-        </is>
-      </c>
-      <c r="D13" t="inlineStr">
-        <is>
-          <t>ranger</t>
-        </is>
-      </c>
-      <c r="E13" t="inlineStr">
-        <is>
-          <t>rangers</t>
-        </is>
+      <c r="B13" t="s">
+        <v>41</v>
+      </c>
+      <c r="C13" t="s">
+        <v>17</v>
+      </c>
+      <c r="D13" t="s">
+        <v>45</v>
+      </c>
+      <c r="E13" t="s">
+        <v>46</v>
       </c>
       <c r="F13" t="n">
         <v>0</v>
@@ -1082,7 +1215,7 @@
         <v>6</v>
       </c>
       <c r="J13" t="n">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="K13" t="n">
         <v>15</v>
@@ -1096,35 +1229,25 @@
       <c r="N13" t="n">
         <v>3</v>
       </c>
-      <c r="O13" t="inlineStr">
-        <is>
-          <t>Excellent offensive troops.</t>
-        </is>
-      </c>
-    </row>
-    <row r="14">
+      <c r="O13" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:15">
       <c r="A14" s="1" t="n">
         <v>12</v>
       </c>
-      <c r="B14" t="inlineStr">
-        <is>
-          <t>Elf</t>
-        </is>
-      </c>
-      <c r="C14" t="inlineStr">
-        <is>
-          <t>archer</t>
-        </is>
-      </c>
-      <c r="D14" t="inlineStr">
-        <is>
-          <t>longbowman</t>
-        </is>
-      </c>
-      <c r="E14" t="inlineStr">
-        <is>
-          <t>longbowmen</t>
-        </is>
+      <c r="B14" t="s">
+        <v>41</v>
+      </c>
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14" t="s">
+        <v>48</v>
+      </c>
+      <c r="E14" t="s">
+        <v>49</v>
       </c>
       <c r="F14" t="n">
         <v>30</v>
@@ -1139,7 +1262,7 @@
         <v>8</v>
       </c>
       <c r="J14" t="n">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="K14" t="n">
         <v>15</v>
@@ -1153,35 +1276,25 @@
       <c r="N14" t="n">
         <v>3</v>
       </c>
-      <c r="O14" t="inlineStr">
-        <is>
-          <t>Longbowmen are very effective at defending your county.</t>
-        </is>
-      </c>
-    </row>
-    <row r="15">
+      <c r="O14" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="15" spans="1:15">
       <c r="A15" s="1" t="n">
         <v>13</v>
       </c>
-      <c r="B15" t="inlineStr">
-        <is>
-          <t>Elf</t>
-        </is>
-      </c>
-      <c r="C15" t="inlineStr">
-        <is>
-          <t>elite</t>
-        </is>
-      </c>
-      <c r="D15" t="inlineStr">
-        <is>
-          <t>dragonhelm</t>
-        </is>
-      </c>
-      <c r="E15" t="inlineStr">
-        <is>
-          <t>dragonhelms</t>
-        </is>
+      <c r="B15" t="s">
+        <v>41</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>51</v>
+      </c>
+      <c r="E15" t="s">
+        <v>52</v>
       </c>
       <c r="F15" t="n">
         <v>0</v>
@@ -1196,7 +1309,7 @@
         <v>15</v>
       </c>
       <c r="J15" t="n">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="K15" t="n">
         <v>25</v>
@@ -1210,35 +1323,25 @@
       <c r="N15" t="n">
         <v>6</v>
       </c>
-      <c r="O15" t="inlineStr">
-        <is>
-          <t>Dragonhelms are elite cavalry and incredibly adept at attacking enemy counties.</t>
-        </is>
-      </c>
-    </row>
-    <row r="16">
+      <c r="O15" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="16" spans="1:15">
       <c r="A16" s="1" t="n">
         <v>14</v>
       </c>
-      <c r="B16" t="inlineStr">
-        <is>
-          <t>Elf</t>
-        </is>
-      </c>
-      <c r="C16" t="inlineStr">
-        <is>
-          <t>monster</t>
-        </is>
-      </c>
-      <c r="D16" t="inlineStr">
-        <is>
-          <t>dragon</t>
-        </is>
-      </c>
-      <c r="E16" t="inlineStr">
-        <is>
-          <t>dragons</t>
-        </is>
+      <c r="B16" t="s">
+        <v>41</v>
+      </c>
+      <c r="C16" t="s">
+        <v>23</v>
+      </c>
+      <c r="D16" t="s">
+        <v>54</v>
+      </c>
+      <c r="E16" t="s">
+        <v>55</v>
       </c>
       <c r="F16" t="n">
         <v>0</v>
@@ -1267,35 +1370,25 @@
       <c r="N16" t="n">
         <v>25</v>
       </c>
-      <c r="O16" t="inlineStr">
-        <is>
-          <t>Dragons are incredibly powerful monsters.</t>
-        </is>
-      </c>
-    </row>
-    <row r="17">
+      <c r="O16" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="17" spans="1:15">
       <c r="A17" s="1" t="n">
         <v>15</v>
       </c>
-      <c r="B17" t="inlineStr">
-        <is>
-          <t>Dwarf</t>
-        </is>
-      </c>
-      <c r="C17" t="inlineStr">
-        <is>
-          <t>peasant</t>
-        </is>
-      </c>
-      <c r="D17" t="inlineStr">
-        <is>
-          <t>miner</t>
-        </is>
-      </c>
-      <c r="E17" t="inlineStr">
-        <is>
-          <t>miners</t>
-        </is>
+      <c r="B17" t="s">
+        <v>57</v>
+      </c>
+      <c r="C17" t="s">
+        <v>14</v>
+      </c>
+      <c r="D17" t="s">
+        <v>58</v>
+      </c>
+      <c r="E17" t="s">
+        <v>59</v>
       </c>
       <c r="F17" t="n">
         <v>25</v>
@@ -1324,35 +1417,25 @@
       <c r="N17" t="n">
         <v>2</v>
       </c>
-      <c r="O17" t="inlineStr">
-        <is>
-          <t>Miners deal extra damage when attacking.</t>
-        </is>
-      </c>
-    </row>
-    <row r="18">
+      <c r="O17" t="s">
+        <v>60</v>
+      </c>
+    </row>
+    <row r="18" spans="1:15">
       <c r="A18" s="1" t="n">
         <v>16</v>
       </c>
-      <c r="B18" t="inlineStr">
-        <is>
-          <t>Dwarf</t>
-        </is>
-      </c>
-      <c r="C18" t="inlineStr">
-        <is>
-          <t>soldier</t>
-        </is>
-      </c>
-      <c r="D18" t="inlineStr">
-        <is>
-          <t>axeman</t>
-        </is>
-      </c>
-      <c r="E18" t="inlineStr">
-        <is>
-          <t>axemen</t>
-        </is>
+      <c r="B18" t="s">
+        <v>57</v>
+      </c>
+      <c r="C18" t="s">
+        <v>17</v>
+      </c>
+      <c r="D18" t="s">
+        <v>61</v>
+      </c>
+      <c r="E18" t="s">
+        <v>62</v>
       </c>
       <c r="F18" t="n">
         <v>0</v>
@@ -1381,35 +1464,25 @@
       <c r="N18" t="n">
         <v>4</v>
       </c>
-      <c r="O18" t="inlineStr">
-        <is>
-          <t>Excellent offensive troops.</t>
-        </is>
-      </c>
-    </row>
-    <row r="19">
+      <c r="O18" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="19" spans="1:15">
       <c r="A19" s="1" t="n">
         <v>17</v>
       </c>
-      <c r="B19" t="inlineStr">
-        <is>
-          <t>Dwarf</t>
-        </is>
-      </c>
-      <c r="C19" t="inlineStr">
-        <is>
-          <t>archer</t>
-        </is>
-      </c>
-      <c r="D19" t="inlineStr">
-        <is>
-          <t>rifleman</t>
-        </is>
-      </c>
-      <c r="E19" t="inlineStr">
-        <is>
-          <t>riflemen</t>
-        </is>
+      <c r="B19" t="s">
+        <v>57</v>
+      </c>
+      <c r="C19" t="s">
+        <v>19</v>
+      </c>
+      <c r="D19" t="s">
+        <v>63</v>
+      </c>
+      <c r="E19" t="s">
+        <v>64</v>
       </c>
       <c r="F19" t="n">
         <v>30</v>
@@ -1438,35 +1511,25 @@
       <c r="N19" t="n">
         <v>4</v>
       </c>
-      <c r="O19" t="inlineStr">
-        <is>
-          <t>Dwarf riflemen are a powerful defensive force.</t>
-        </is>
-      </c>
-    </row>
-    <row r="20">
+      <c r="O19" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="20" spans="1:15">
       <c r="A20" s="1" t="n">
         <v>18</v>
       </c>
-      <c r="B20" t="inlineStr">
-        <is>
-          <t>Dwarf</t>
-        </is>
-      </c>
-      <c r="C20" t="inlineStr">
-        <is>
-          <t>elite</t>
-        </is>
-      </c>
-      <c r="D20" t="inlineStr">
-        <is>
-          <t>greybeard</t>
-        </is>
-      </c>
-      <c r="E20" t="inlineStr">
-        <is>
-          <t>greybeards</t>
-        </is>
+      <c r="B20" t="s">
+        <v>57</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>66</v>
+      </c>
+      <c r="E20" t="s">
+        <v>67</v>
       </c>
       <c r="F20" t="n">
         <v>0</v>
@@ -1495,35 +1558,25 @@
       <c r="N20" t="n">
         <v>8</v>
       </c>
-      <c r="O20" t="inlineStr">
-        <is>
-          <t>Greybeards are capable of defending, as well as attacking.</t>
-        </is>
-      </c>
-    </row>
-    <row r="21">
+      <c r="O20" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="21" spans="1:15">
       <c r="A21" s="1" t="n">
         <v>19</v>
       </c>
-      <c r="B21" t="inlineStr">
-        <is>
-          <t>Dwarf</t>
-        </is>
-      </c>
-      <c r="C21" t="inlineStr">
-        <is>
-          <t>monster</t>
-        </is>
-      </c>
-      <c r="D21" t="inlineStr">
-        <is>
-          <t>manticore</t>
-        </is>
-      </c>
-      <c r="E21" t="inlineStr">
-        <is>
-          <t>manticores</t>
-        </is>
+      <c r="B21" t="s">
+        <v>57</v>
+      </c>
+      <c r="C21" t="s">
+        <v>23</v>
+      </c>
+      <c r="D21" t="s">
+        <v>69</v>
+      </c>
+      <c r="E21" t="s">
+        <v>70</v>
       </c>
       <c r="F21" t="n">
         <v>0</v>
@@ -1552,35 +1605,25 @@
       <c r="N21" t="n">
         <v>25</v>
       </c>
-      <c r="O21" t="inlineStr">
-        <is>
-          <t>Manticores are incredibly powerful monsters.</t>
-        </is>
-      </c>
-    </row>
-    <row r="22">
+      <c r="O21" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="22" spans="1:15">
       <c r="A22" s="1" t="n">
         <v>20</v>
       </c>
-      <c r="B22" t="inlineStr">
-        <is>
-          <t>Goblin</t>
-        </is>
-      </c>
-      <c r="C22" t="inlineStr">
-        <is>
-          <t>peasant</t>
-        </is>
-      </c>
-      <c r="D22" t="inlineStr">
-        <is>
-          <t>scout</t>
-        </is>
-      </c>
-      <c r="E22" t="inlineStr">
-        <is>
-          <t>scouts</t>
-        </is>
+      <c r="B22" t="s">
+        <v>72</v>
+      </c>
+      <c r="C22" t="s">
+        <v>14</v>
+      </c>
+      <c r="D22" t="s">
+        <v>73</v>
+      </c>
+      <c r="E22" t="s">
+        <v>74</v>
       </c>
       <c r="F22" t="n">
         <v>25</v>
@@ -1609,35 +1652,25 @@
       <c r="N22" t="n">
         <v>1</v>
       </c>
-      <c r="O22" t="inlineStr">
-        <is>
-          <t>Scouts are cheap and expendable.</t>
-        </is>
-      </c>
-    </row>
-    <row r="23">
+      <c r="O22" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="23" spans="1:15">
       <c r="A23" s="1" t="n">
         <v>21</v>
       </c>
-      <c r="B23" t="inlineStr">
-        <is>
-          <t>Goblin</t>
-        </is>
-      </c>
-      <c r="C23" t="inlineStr">
-        <is>
-          <t>soldier</t>
-        </is>
-      </c>
-      <c r="D23" t="inlineStr">
-        <is>
-          <t>berserker</t>
-        </is>
-      </c>
-      <c r="E23" t="inlineStr">
-        <is>
-          <t>berserkers</t>
-        </is>
+      <c r="B23" t="s">
+        <v>72</v>
+      </c>
+      <c r="C23" t="s">
+        <v>17</v>
+      </c>
+      <c r="D23" t="s">
+        <v>76</v>
+      </c>
+      <c r="E23" t="s">
+        <v>77</v>
       </c>
       <c r="F23" t="n">
         <v>0</v>
@@ -1666,35 +1699,25 @@
       <c r="N23" t="n">
         <v>2</v>
       </c>
-      <c r="O23" t="inlineStr">
-        <is>
-          <t>Soldiers are a solid offensive troop.</t>
-        </is>
-      </c>
-    </row>
-    <row r="24">
+      <c r="O23" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="24" spans="1:15">
       <c r="A24" s="1" t="n">
         <v>22</v>
       </c>
-      <c r="B24" t="inlineStr">
-        <is>
-          <t>Goblin</t>
-        </is>
-      </c>
-      <c r="C24" t="inlineStr">
-        <is>
-          <t>archer</t>
-        </is>
-      </c>
-      <c r="D24" t="inlineStr">
-        <is>
-          <t>bowman</t>
-        </is>
-      </c>
-      <c r="E24" t="inlineStr">
-        <is>
-          <t>bowmen</t>
-        </is>
+      <c r="B24" t="s">
+        <v>72</v>
+      </c>
+      <c r="C24" t="s">
+        <v>19</v>
+      </c>
+      <c r="D24" t="s">
+        <v>79</v>
+      </c>
+      <c r="E24" t="s">
+        <v>80</v>
       </c>
       <c r="F24" t="n">
         <v>35</v>
@@ -1723,35 +1746,25 @@
       <c r="N24" t="n">
         <v>3</v>
       </c>
-      <c r="O24" t="inlineStr">
-        <is>
-          <t>Goblin archers are weaker than other archers but much cheaper.</t>
-        </is>
-      </c>
-    </row>
-    <row r="25">
+      <c r="O24" t="s">
+        <v>81</v>
+      </c>
+    </row>
+    <row r="25" spans="1:15">
       <c r="A25" s="1" t="n">
         <v>23</v>
       </c>
-      <c r="B25" t="inlineStr">
-        <is>
-          <t>Goblin</t>
-        </is>
-      </c>
-      <c r="C25" t="inlineStr">
-        <is>
-          <t>elite</t>
-        </is>
-      </c>
-      <c r="D25" t="inlineStr">
-        <is>
-          <t>wolf rider</t>
-        </is>
-      </c>
-      <c r="E25" t="inlineStr">
-        <is>
-          <t>wolf riders</t>
-        </is>
+      <c r="B25" t="s">
+        <v>72</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>82</v>
+      </c>
+      <c r="E25" t="s">
+        <v>83</v>
       </c>
       <c r="F25" t="n">
         <v>0</v>
@@ -1780,35 +1793,25 @@
       <c r="N25" t="n">
         <v>5</v>
       </c>
-      <c r="O25" t="inlineStr">
-        <is>
-          <t>In large numbers, wolf riders are incredibly powerful.</t>
-        </is>
-      </c>
-    </row>
-    <row r="26">
+      <c r="O25" t="s">
+        <v>84</v>
+      </c>
+    </row>
+    <row r="26" spans="1:15">
       <c r="A26" s="1" t="n">
         <v>24</v>
       </c>
-      <c r="B26" t="inlineStr">
-        <is>
-          <t>Goblin</t>
-        </is>
-      </c>
-      <c r="C26" t="inlineStr">
-        <is>
-          <t>monster</t>
-        </is>
-      </c>
-      <c r="D26" t="inlineStr">
-        <is>
-          <t>wyvern</t>
-        </is>
-      </c>
-      <c r="E26" t="inlineStr">
-        <is>
-          <t>wyverns</t>
-        </is>
+      <c r="B26" t="s">
+        <v>72</v>
+      </c>
+      <c r="C26" t="s">
+        <v>23</v>
+      </c>
+      <c r="D26" t="s">
+        <v>85</v>
+      </c>
+      <c r="E26" t="s">
+        <v>86</v>
       </c>
       <c r="F26" t="n">
         <v>0</v>
@@ -1837,10 +1840,8 @@
       <c r="N26" t="n">
         <v>25</v>
       </c>
-      <c r="O26" t="inlineStr">
-        <is>
-          <t>Wyverns are devastating to any who cross their path.</t>
-        </is>
+      <c r="O26" t="s">
+        <v>87</v>
       </c>
     </row>
   </sheetData>

</xml_diff>